<commit_message>
modular text buttpons established with documentation.
</commit_message>
<xml_diff>
--- a/admin/Timesheets/Caroline Chang/Week 22 Timesheet.xlsx
+++ b/admin/Timesheets/Caroline Chang/Week 22 Timesheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\carol\CSCI_Classes\CSCI4308\capstone_proj\admin\Timesheets\Caroline Chang\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9FE3FF5-7B59-4351-9C8B-2C51471B9CC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{313D655A-8DC9-4F26-B7D6-1B804E60DD04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -427,7 +427,7 @@
   <dimension ref="A4:K14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K15" sqref="K15"/>
+      <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -530,8 +530,11 @@
       <c r="B13">
         <v>2</v>
       </c>
+      <c r="D13">
+        <v>2</v>
+      </c>
       <c r="I13" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.3">
@@ -542,13 +545,15 @@
         <v>2</v>
       </c>
       <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
+      <c r="D14" s="1">
+        <v>2</v>
+      </c>
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
       <c r="G14" s="1"/>
       <c r="H14" s="1"/>
       <c r="I14" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
transitions between different views completed.
</commit_message>
<xml_diff>
--- a/admin/Timesheets/Caroline Chang/Week 22 Timesheet.xlsx
+++ b/admin/Timesheets/Caroline Chang/Week 22 Timesheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\carol\CSCI_Classes\CSCI4308\capstone_proj\admin\Timesheets\Caroline Chang\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{313D655A-8DC9-4F26-B7D6-1B804E60DD04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A404497E-D0E6-4A91-A8F6-F6C0B29DC512}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -427,7 +427,7 @@
   <dimension ref="A4:K14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K14" sqref="K14"/>
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -497,13 +497,23 @@
       <c r="A8" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="I8" s="1"/>
+      <c r="D8">
+        <v>0.5</v>
+      </c>
+      <c r="I8" s="1">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="I9" s="1"/>
+      <c r="D9">
+        <v>0.5</v>
+      </c>
+      <c r="I9" s="1">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
@@ -533,8 +543,11 @@
       <c r="D13">
         <v>2</v>
       </c>
+      <c r="E13">
+        <v>1</v>
+      </c>
       <c r="I13" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.3">
@@ -546,14 +559,16 @@
       </c>
       <c r="C14" s="1"/>
       <c r="D14" s="1">
-        <v>2</v>
-      </c>
-      <c r="E14" s="1"/>
+        <v>3</v>
+      </c>
+      <c r="E14" s="1">
+        <v>1</v>
+      </c>
       <c r="F14" s="1"/>
       <c r="G14" s="1"/>
       <c r="H14" s="1"/>
       <c r="I14" s="1">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>